<commit_message>
changes to make PAMless run smoother
Added parameter to select if looking for PAMless guides. Updated FindCC and FindGG functions to take this parameter into account. Update guide selection so that PAMless will randomly select n top hits (default NGG will select first n hits ordered by location). Added if statement so that a list of promoter guides is only made if there is at least one promoter guide.
</commit_message>
<xml_diff>
--- a/GuideFinder-Mac/E_coli_DH5alpha/Pasteur_ftsz_predicted_guides.xlsx
+++ b/GuideFinder-Mac/E_coli_DH5alpha/Pasteur_ftsz_predicted_guides.xlsx
@@ -1,21 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mellos/Documents/GitHub/Guide-Finder/GuideFinder-Mac/E_coli_DH5alpha/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8687041A-B9B0-0B46-A7AC-E56E1CDBAF36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D7DA146-37F0-2445-B9A4-5F148FBA2F73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35660" yWindow="-2380" windowWidth="15960" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10080" yWindow="500" windowWidth="15960" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1 - CRISPR Pasteur - brow" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -172,6 +185,7 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -326,10 +340,10 @@
     </xf>
   </cellStyleXfs>
   <cellXfs count="11">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -338,19 +352,19 @@
     <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1522,7 +1536,7 @@
   <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>